<commit_message>
search - in progress
</commit_message>
<xml_diff>
--- a/doc/FEATURES_ROADMAP_03.xlsx
+++ b/doc/FEATURES_ROADMAP_03.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="176">
   <si>
     <t>mechanizm lockowania dokumentów</t>
   </si>
@@ -643,6 +643,18 @@
   </si>
   <si>
     <t>Elastic search, Kibana, full-text search</t>
+  </si>
+  <si>
+    <t>FILE OPERATIONS</t>
+  </si>
+  <si>
+    <t>zip operations</t>
+  </si>
+  <si>
+    <t>file upload / download</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -1250,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K109"/>
+  <dimension ref="B1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1369,7 +1381,9 @@
       <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1493,12 +1507,12 @@
       <c r="E17" t="s">
         <v>147</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" s="3" t="s">
@@ -1596,6 +1610,16 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="F25" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" s="3" t="s">
@@ -1692,7 +1716,9 @@
       <c r="E33" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1906,6 +1932,9 @@
       <c r="K49" s="7"/>
     </row>
     <row r="50" spans="2:11">
+      <c r="E50" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
@@ -1913,57 +1942,55 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
+    <row r="51" spans="2:11">
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>174</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
     <row r="52" spans="2:11">
-      <c r="B52" s="3" t="s">
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>173</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="54" spans="2:11">
+      <c r="B54" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>71</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="53" spans="2:11">
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
-        <v>49</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-    </row>
-    <row r="54" spans="2:11">
-      <c r="D54">
-        <v>2</v>
-      </c>
-      <c r="E54" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
     </row>
     <row r="55" spans="2:11">
       <c r="D55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -1972,12 +1999,14 @@
     </row>
     <row r="56" spans="2:11">
       <c r="D56">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>83</v>
-      </c>
-      <c r="F56" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -1986,10 +2015,10 @@
     </row>
     <row r="57" spans="2:11">
       <c r="D57">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -1999,58 +2028,58 @@
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="2:11">
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
+      <c r="D58">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
     </row>
     <row r="59" spans="2:11">
-      <c r="E59" s="2" t="s">
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>163</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="2:11">
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+    </row>
+    <row r="61" spans="2:11">
+      <c r="E61" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-    </row>
-    <row r="60" spans="2:11">
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>167</v>
-      </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-    </row>
-    <row r="61" spans="2:11">
-      <c r="D61">
-        <v>2</v>
-      </c>
-      <c r="E61" t="s">
-        <v>153</v>
-      </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
     </row>
     <row r="62" spans="2:11">
       <c r="D62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -2061,10 +2090,10 @@
     </row>
     <row r="63" spans="2:11">
       <c r="D63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -2075,10 +2104,10 @@
     </row>
     <row r="64" spans="2:11">
       <c r="D64">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -2089,10 +2118,10 @@
     </row>
     <row r="65" spans="2:11">
       <c r="D65">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2103,63 +2132,63 @@
     </row>
     <row r="66" spans="2:11">
       <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>151</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="D67">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>152</v>
+      </c>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+    </row>
+    <row r="68" spans="2:11">
+      <c r="D68">
         <v>7</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E68" t="s">
         <v>164</v>
       </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
-    </row>
-    <row r="68" spans="2:11">
-      <c r="B68" s="3" t="s">
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="70" spans="2:11">
+      <c r="B70" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C70" t="s">
         <v>81</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="69" spans="2:11">
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69" t="s">
-        <v>79</v>
-      </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-    </row>
-    <row r="70" spans="2:11">
-      <c r="D70">
-        <v>2</v>
-      </c>
-      <c r="E70" t="s">
-        <v>78</v>
-      </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
     </row>
     <row r="71" spans="2:11">
       <c r="D71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>144</v>
+        <v>79</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2170,10 +2199,10 @@
     </row>
     <row r="72" spans="2:11">
       <c r="D72">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -2184,10 +2213,10 @@
     </row>
     <row r="73" spans="2:11">
       <c r="D73">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E73" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -2196,90 +2225,90 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
+    <row r="74" spans="2:11">
+      <c r="D74">
+        <v>4</v>
+      </c>
+      <c r="E74" t="s">
+        <v>77</v>
+      </c>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+    </row>
     <row r="75" spans="2:11">
-      <c r="B75" s="3" t="s">
+      <c r="D75">
+        <v>5</v>
+      </c>
+      <c r="E75" t="s">
+        <v>80</v>
+      </c>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+    </row>
+    <row r="77" spans="2:11">
+      <c r="B77" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>72</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E77" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="2:11">
-      <c r="D76">
+    <row r="78" spans="2:11">
+      <c r="D78">
         <v>1</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E78" t="s">
         <v>75</v>
       </c>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-    </row>
-    <row r="77" spans="2:11">
-      <c r="D77">
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+    </row>
+    <row r="79" spans="2:11">
+      <c r="D79">
         <v>2</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E79" t="s">
         <v>66</v>
       </c>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-    </row>
-    <row r="79" spans="2:11">
-      <c r="B79" s="3" t="s">
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+    </row>
+    <row r="81" spans="2:11">
+      <c r="B81" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>62</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="80" spans="2:11">
-      <c r="D80">
-        <v>1</v>
-      </c>
-      <c r="E80" t="s">
-        <v>52</v>
-      </c>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-    </row>
-    <row r="81" spans="2:11">
-      <c r="D81">
-        <v>2</v>
-      </c>
-      <c r="E81" t="s">
-        <v>53</v>
-      </c>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
     </row>
     <row r="82" spans="2:11">
       <c r="D82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -2288,51 +2317,51 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
+    <row r="83" spans="2:11">
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s">
+        <v>53</v>
+      </c>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+    </row>
     <row r="84" spans="2:11">
-      <c r="B84" s="3" t="s">
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84" t="s">
+        <v>54</v>
+      </c>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="86" spans="2:11">
+      <c r="B86" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>73</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="85" spans="2:11">
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" t="s">
-        <v>58</v>
-      </c>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-    </row>
-    <row r="86" spans="2:11">
-      <c r="D86">
-        <v>2</v>
-      </c>
-      <c r="E86" t="s">
-        <v>59</v>
-      </c>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
     </row>
     <row r="87" spans="2:11">
       <c r="D87">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
@@ -2341,51 +2370,51 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
+    <row r="88" spans="2:11">
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88" t="s">
+        <v>59</v>
+      </c>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+    </row>
     <row r="89" spans="2:11">
-      <c r="B89" s="3" t="s">
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89" t="s">
+        <v>60</v>
+      </c>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+    </row>
+    <row r="91" spans="2:11">
+      <c r="B91" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C91" t="s">
         <v>65</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E91" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="90" spans="2:11">
-      <c r="D90">
-        <v>1</v>
-      </c>
-      <c r="E90" t="s">
-        <v>157</v>
-      </c>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-    </row>
-    <row r="91" spans="2:11">
-      <c r="D91">
-        <v>2</v>
-      </c>
-      <c r="E91" t="s">
-        <v>85</v>
-      </c>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1"/>
     </row>
     <row r="92" spans="2:11">
       <c r="D92">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
@@ -2396,33 +2425,39 @@
     </row>
     <row r="93" spans="2:11">
       <c r="D93">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>155</v>
-      </c>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="7"/>
-      <c r="J93" s="7"/>
-      <c r="K93" s="7"/>
+        <v>85</v>
+      </c>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
     </row>
     <row r="94" spans="2:11">
       <c r="D94">
-        <v>5</v>
-      </c>
-      <c r="E94" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="E94" t="s">
+        <v>86</v>
+      </c>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
     </row>
     <row r="95" spans="2:11">
+      <c r="D95">
+        <v>4</v>
+      </c>
+      <c r="E95" t="s">
+        <v>155</v>
+      </c>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
@@ -2431,6 +2466,12 @@
       <c r="K95" s="7"/>
     </row>
     <row r="96" spans="2:11">
+      <c r="D96">
+        <v>5</v>
+      </c>
+      <c r="E96" s="37" t="s">
+        <v>156</v>
+      </c>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
@@ -2438,67 +2479,83 @@
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
     </row>
-    <row r="97" spans="3:9">
-      <c r="C97" s="4" t="s">
+    <row r="97" spans="3:11">
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+    </row>
+    <row r="98" spans="3:11">
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
+      <c r="I98" s="7"/>
+      <c r="J98" s="7"/>
+      <c r="K98" s="7"/>
+    </row>
+    <row r="99" spans="3:11">
+      <c r="C99" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4" t="s">
+      <c r="D99" s="4"/>
+      <c r="E99" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="3:9">
-      <c r="C98" s="4" t="s">
+    <row r="100" spans="3:11">
+      <c r="C100" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4" t="s">
+      <c r="D100" s="4"/>
+      <c r="E100" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="3:9">
-      <c r="C100" t="s">
+    <row r="102" spans="3:11">
+      <c r="C102" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="103" spans="3:9">
-      <c r="C103" t="s">
+    <row r="105" spans="3:11">
+      <c r="C105" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="3:9">
-      <c r="C104" t="s">
+    <row r="106" spans="3:11">
+      <c r="C106" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="3:9">
-      <c r="C105" t="s">
+    <row r="107" spans="3:11">
+      <c r="C107" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="3:9">
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
-      <c r="I106" s="1"/>
-    </row>
-    <row r="107" spans="3:9" ht="24" customHeight="1">
-      <c r="C107" t="s">
+    <row r="108" spans="3:11">
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+    </row>
+    <row r="109" spans="3:11" ht="24" customHeight="1">
+      <c r="C109" t="s">
         <v>103</v>
       </c>
-      <c r="G107" s="11"/>
-      <c r="H107" s="12"/>
-      <c r="I107" s="13"/>
-    </row>
-    <row r="108" spans="3:9" ht="34.200000000000003" customHeight="1">
-      <c r="C108" t="s">
+      <c r="G109" s="11"/>
+      <c r="H109" s="12"/>
+      <c r="I109" s="13"/>
+    </row>
+    <row r="110" spans="3:11" ht="34.200000000000003" customHeight="1">
+      <c r="C110" t="s">
         <v>104</v>
       </c>
-      <c r="G108" s="11"/>
-      <c r="H108" s="12"/>
-      <c r="I108" s="13"/>
-    </row>
-    <row r="109" spans="3:9">
-      <c r="C109" t="s">
+      <c r="G110" s="11"/>
+      <c r="H110" s="12"/>
+      <c r="I110" s="13"/>
+    </row>
+    <row r="111" spans="3:11">
+      <c r="C111" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusted to UI tests
</commit_message>
<xml_diff>
--- a/doc/FEATURES_ROADMAP_03.xlsx
+++ b/doc/FEATURES_ROADMAP_03.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="175">
   <si>
     <t>mechanizm lockowania dokumentów</t>
   </si>
@@ -637,6 +637,21 @@
   </si>
   <si>
     <t xml:space="preserve"> - tests based on c service project (config, sql inserts, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - run simple ui test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - login to application</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - locate compoents by x-path various examples</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - assertions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - db queries and tests</t>
   </si>
 </sst>
 </file>
@@ -1255,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2331,7 +2346,7 @@
         <v>73</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -2340,14 +2355,11 @@
       <c r="K79" s="1"/>
     </row>
     <row r="80" spans="2:11">
-      <c r="D80">
-        <v>2</v>
-      </c>
       <c r="E80" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
@@ -2355,26 +2367,38 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
+    <row r="81" spans="2:11">
+      <c r="E81" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+    </row>
     <row r="82" spans="2:11">
-      <c r="B82" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" t="s">
-        <v>60</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="E82" t="s">
+        <v>172</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
     </row>
     <row r="83" spans="2:11">
-      <c r="D83">
-        <v>1</v>
-      </c>
       <c r="E83" t="s">
-        <v>50</v>
+        <v>173</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -2383,14 +2407,11 @@
       <c r="K83" s="1"/>
     </row>
     <row r="84" spans="2:11">
-      <c r="D84">
-        <v>2</v>
-      </c>
       <c r="E84" t="s">
-        <v>51</v>
+        <v>174</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
@@ -2398,55 +2419,39 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="2:11">
-      <c r="D85">
-        <v>3</v>
-      </c>
-      <c r="E85" t="s">
-        <v>52</v>
-      </c>
-      <c r="F85" s="1" t="s">
+    <row r="86" spans="2:11">
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
+        <v>64</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-    </row>
-    <row r="87" spans="2:11">
-      <c r="B87" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C87" t="s">
-        <v>71</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
     </row>
     <row r="88" spans="2:11">
-      <c r="D88">
-        <v>1</v>
-      </c>
-      <c r="E88" t="s">
-        <v>56</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
+      <c r="B88" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C88" t="s">
+        <v>60</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="89" spans="2:11">
       <c r="D89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>22</v>
@@ -2459,10 +2464,10 @@
     </row>
     <row r="90" spans="2:11">
       <c r="D90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>22</v>
@@ -2473,39 +2478,39 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="92" spans="2:11">
-      <c r="B92" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C92" t="s">
-        <v>63</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>145</v>
-      </c>
+    <row r="91" spans="2:11">
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91" t="s">
+        <v>52</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
     </row>
     <row r="93" spans="2:11">
-      <c r="D93">
-        <v>1</v>
-      </c>
-      <c r="E93" t="s">
-        <v>148</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
+      <c r="B93" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C93" t="s">
+        <v>71</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="94" spans="2:11">
       <c r="D94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>22</v>
@@ -2518,10 +2523,10 @@
     </row>
     <row r="95" spans="2:11">
       <c r="D95">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E95" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>22</v>
@@ -2534,10 +2539,10 @@
     </row>
     <row r="96" spans="2:11">
       <c r="D96">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E96" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>22</v>
@@ -2548,93 +2553,156 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="3:11">
-      <c r="D97">
+    <row r="98" spans="2:11">
+      <c r="B98" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C98" t="s">
+        <v>63</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11">
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99" t="s">
+        <v>148</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+    </row>
+    <row r="100" spans="2:11">
+      <c r="D100">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s">
+        <v>83</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+    </row>
+    <row r="101" spans="2:11">
+      <c r="D101">
+        <v>3</v>
+      </c>
+      <c r="E101" t="s">
+        <v>84</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+    </row>
+    <row r="102" spans="2:11">
+      <c r="D102">
+        <v>4</v>
+      </c>
+      <c r="E102" t="s">
+        <v>146</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+    </row>
+    <row r="103" spans="2:11">
+      <c r="D103">
         <v>5</v>
       </c>
-      <c r="E97" s="37" t="s">
+      <c r="E103" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="F97" s="1" t="s">
+      <c r="F103" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
-      <c r="K97" s="1"/>
-    </row>
-    <row r="98" spans="3:11">
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
-      <c r="I98" s="7"/>
-      <c r="J98" s="7"/>
-      <c r="K98" s="7"/>
-    </row>
-    <row r="99" spans="3:11">
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
-      <c r="I99" s="7"/>
-      <c r="J99" s="7"/>
-      <c r="K99" s="7"/>
-    </row>
-    <row r="100" spans="3:11">
-      <c r="C100" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4" t="s">
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+    </row>
+    <row r="104" spans="2:11">
+      <c r="F104" s="7"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
+    </row>
+    <row r="105" spans="2:11">
+      <c r="F105" s="7"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+    </row>
+    <row r="106" spans="2:11">
+      <c r="C106" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="3:11">
-      <c r="C101" s="4" t="s">
+    <row r="107" spans="2:11">
+      <c r="C107" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D101" s="4"/>
-      <c r="E101" s="4" t="s">
+      <c r="D107" s="4"/>
+      <c r="E107" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="3:11">
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
-      <c r="H106" s="7"/>
-      <c r="I106" s="7"/>
-    </row>
-    <row r="107" spans="3:11">
-      <c r="F107" s="7"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="7"/>
-      <c r="I107" s="7"/>
-    </row>
-    <row r="108" spans="3:11">
+    <row r="108" spans="2:11">
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
     </row>
-    <row r="109" spans="3:11">
+    <row r="109" spans="2:11">
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
     </row>
-    <row r="110" spans="3:11">
+    <row r="110" spans="2:11">
       <c r="F110" s="7"/>
       <c r="G110" s="38"/>
       <c r="H110" s="39"/>
       <c r="I110" s="40"/>
     </row>
-    <row r="111" spans="3:11">
+    <row r="111" spans="2:11">
       <c r="F111" s="7"/>
       <c r="G111" s="38"/>
       <c r="H111" s="39"/>
       <c r="I111" s="40"/>
     </row>
-    <row r="112" spans="3:11">
+    <row r="112" spans="2:11">
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>

</xml_diff>

<commit_message>
Added email impl - in progress
</commit_message>
<xml_diff>
--- a/doc/FEATURES_ROADMAP_03.xlsx
+++ b/doc/FEATURES_ROADMAP_03.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="177">
   <si>
     <t>mechanizm lockowania dokumentów</t>
   </si>
@@ -652,6 +652,12 @@
   </si>
   <si>
     <t xml:space="preserve"> - db queries and tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - account management, create user, reset pass etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - main menu bar</t>
   </si>
 </sst>
 </file>
@@ -749,7 +755,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -900,11 +906,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -974,6 +991,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1270,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1871,50 +1890,45 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
+    <row r="43" spans="2:11">
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
     <row r="44" spans="2:11">
-      <c r="B44" s="3" t="s">
+      <c r="D44">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F44" s="41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>86</v>
       </c>
-      <c r="D44">
+      <c r="D46">
         <v>1</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="2:11">
-      <c r="D45">
-        <v>2</v>
-      </c>
-      <c r="E45" t="s">
-        <v>72</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-    </row>
-    <row r="46" spans="2:11">
-      <c r="D46">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>45</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>16</v>
@@ -1927,10 +1941,10 @@
     </row>
     <row r="47" spans="2:11">
       <c r="D47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>152</v>
+        <v>72</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>16</v>
@@ -1943,13 +1957,13 @@
     </row>
     <row r="48" spans="2:11">
       <c r="D48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -1959,13 +1973,13 @@
     </row>
     <row r="49" spans="2:11">
       <c r="D49">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E49" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -1974,103 +1988,105 @@
       <c r="K49" s="1"/>
     </row>
     <row r="50" spans="2:11">
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
     </row>
     <row r="51" spans="2:11">
-      <c r="E51" s="2" t="s">
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>150</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="2:11">
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+    </row>
+    <row r="53" spans="2:11">
+      <c r="E53" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-    </row>
-    <row r="52" spans="2:11">
-      <c r="D52">
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="2:11">
+      <c r="D54">
         <v>1</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E54" t="s">
         <v>164</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-    </row>
-    <row r="53" spans="2:11">
-      <c r="D53">
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="2:11">
+      <c r="D55">
         <v>2</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E55" t="s">
         <v>163</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-    </row>
-    <row r="55" spans="2:11">
-      <c r="B55" s="3" t="s">
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="57" spans="2:11">
+      <c r="B57" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="56" spans="2:11">
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" t="s">
-        <v>47</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-    </row>
-    <row r="57" spans="2:11">
-      <c r="D57">
-        <v>2</v>
-      </c>
-      <c r="E57" t="s">
-        <v>48</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
     </row>
     <row r="58" spans="2:11">
       <c r="D58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>49</v>
-      </c>
-      <c r="F58" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -2079,12 +2095,14 @@
     </row>
     <row r="59" spans="2:11">
       <c r="D59">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>81</v>
-      </c>
-      <c r="F59" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -2093,12 +2111,14 @@
     </row>
     <row r="60" spans="2:11">
       <c r="D60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>153</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -2106,62 +2126,62 @@
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="2:11">
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
+      <c r="D61">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
     </row>
     <row r="62" spans="2:11">
-      <c r="E62" s="2" t="s">
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>153</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="2:11">
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" spans="2:11">
+      <c r="E64" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63" t="s">
-        <v>157</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-    </row>
-    <row r="64" spans="2:11">
-      <c r="D64">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s">
-        <v>144</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
     </row>
     <row r="65" spans="2:11">
       <c r="D65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>22</v>
@@ -2174,10 +2194,10 @@
     </row>
     <row r="66" spans="2:11">
       <c r="D66">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>22</v>
@@ -2190,10 +2210,10 @@
     </row>
     <row r="67" spans="2:11">
       <c r="D67">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E67" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>22</v>
@@ -2206,10 +2226,10 @@
     </row>
     <row r="68" spans="2:11">
       <c r="D68">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>22</v>
@@ -2222,10 +2242,10 @@
     </row>
     <row r="69" spans="2:11">
       <c r="D69">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E69" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>22</v>
@@ -2236,55 +2256,55 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
+    <row r="70" spans="2:11">
+      <c r="D70">
+        <v>6</v>
+      </c>
+      <c r="E70" t="s">
+        <v>143</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+    </row>
     <row r="71" spans="2:11">
-      <c r="B71" s="3" t="s">
+      <c r="D71">
+        <v>7</v>
+      </c>
+      <c r="E71" t="s">
+        <v>154</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+    </row>
+    <row r="73" spans="2:11">
+      <c r="B73" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>79</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="72" spans="2:11">
-      <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="E72" t="s">
-        <v>77</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-    </row>
-    <row r="73" spans="2:11">
-      <c r="D73">
-        <v>2</v>
-      </c>
-      <c r="E73" t="s">
-        <v>76</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
     </row>
     <row r="74" spans="2:11">
       <c r="D74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>169</v>
+        <v>77</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>22</v>
@@ -2297,10 +2317,10 @@
     </row>
     <row r="75" spans="2:11">
       <c r="D75">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>22</v>
@@ -2313,10 +2333,10 @@
     </row>
     <row r="76" spans="2:11">
       <c r="D76">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E76" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>22</v>
@@ -2327,49 +2347,55 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
+    <row r="77" spans="2:11">
+      <c r="D77">
+        <v>4</v>
+      </c>
+      <c r="E77" t="s">
+        <v>75</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+    </row>
     <row r="78" spans="2:11">
-      <c r="B78" s="3" t="s">
+      <c r="D78">
+        <v>5</v>
+      </c>
+      <c r="E78" t="s">
+        <v>78</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+    </row>
+    <row r="80" spans="2:11">
+      <c r="B80" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C80" t="s">
         <v>70</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="2:11">
-      <c r="D79">
+    <row r="81" spans="2:11">
+      <c r="D81">
         <v>1</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E81" t="s">
         <v>73</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-    </row>
-    <row r="80" spans="2:11">
-      <c r="E80" t="s">
-        <v>171</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-    </row>
-    <row r="81" spans="2:11">
-      <c r="E81" t="s">
-        <v>170</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>16</v>
@@ -2382,10 +2408,10 @@
     </row>
     <row r="82" spans="2:11">
       <c r="E82" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
@@ -2395,10 +2421,10 @@
     </row>
     <row r="83" spans="2:11">
       <c r="E83" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -2408,7 +2434,7 @@
     </row>
     <row r="84" spans="2:11">
       <c r="E84" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>17</v>
@@ -2419,15 +2445,25 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
+    <row r="85" spans="2:11">
+      <c r="E85" t="s">
+        <v>173</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+    </row>
     <row r="86" spans="2:11">
-      <c r="D86">
-        <v>2</v>
-      </c>
       <c r="E86" t="s">
-        <v>64</v>
+        <v>174</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
@@ -2436,54 +2472,38 @@
       <c r="K86" s="1"/>
     </row>
     <row r="88" spans="2:11">
-      <c r="B88" s="3" t="s">
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88" t="s">
+        <v>64</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+    </row>
+    <row r="90" spans="2:11">
+      <c r="B90" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>60</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E90" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="89" spans="2:11">
-      <c r="D89">
-        <v>1</v>
-      </c>
-      <c r="E89" t="s">
-        <v>50</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
-    </row>
-    <row r="90" spans="2:11">
-      <c r="D90">
-        <v>2</v>
-      </c>
-      <c r="E90" t="s">
-        <v>51</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
     </row>
     <row r="91" spans="2:11">
       <c r="D91">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>22</v>
@@ -2494,55 +2514,55 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
+    <row r="92" spans="2:11">
+      <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92" t="s">
+        <v>51</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+    </row>
     <row r="93" spans="2:11">
-      <c r="B93" s="3" t="s">
+      <c r="D93">
+        <v>3</v>
+      </c>
+      <c r="E93" t="s">
+        <v>52</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="95" spans="2:11">
+      <c r="B95" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C95" t="s">
         <v>71</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="E95" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="94" spans="2:11">
-      <c r="D94">
-        <v>1</v>
-      </c>
-      <c r="E94" t="s">
-        <v>56</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-      <c r="K94" s="1"/>
-    </row>
-    <row r="95" spans="2:11">
-      <c r="D95">
-        <v>2</v>
-      </c>
-      <c r="E95" t="s">
-        <v>57</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
     </row>
     <row r="96" spans="2:11">
       <c r="D96">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>22</v>
@@ -2553,55 +2573,55 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
+    <row r="97" spans="2:11">
+      <c r="D97">
+        <v>2</v>
+      </c>
+      <c r="E97" t="s">
+        <v>57</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
     <row r="98" spans="2:11">
-      <c r="B98" s="3" t="s">
+      <c r="D98">
+        <v>3</v>
+      </c>
+      <c r="E98" t="s">
+        <v>58</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+    </row>
+    <row r="100" spans="2:11">
+      <c r="B100" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C100" t="s">
         <v>63</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="E100" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="99" spans="2:11">
-      <c r="D99">
-        <v>1</v>
-      </c>
-      <c r="E99" t="s">
-        <v>148</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
-      <c r="K99" s="1"/>
-    </row>
-    <row r="100" spans="2:11">
-      <c r="D100">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s">
-        <v>83</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
     </row>
     <row r="101" spans="2:11">
       <c r="D101">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>84</v>
+        <v>148</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>22</v>
@@ -2614,10 +2634,10 @@
     </row>
     <row r="102" spans="2:11">
       <c r="D102">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>146</v>
+        <v>83</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>22</v>
@@ -2630,10 +2650,10 @@
     </row>
     <row r="103" spans="2:11">
       <c r="D103">
-        <v>5</v>
-      </c>
-      <c r="E103" s="37" t="s">
-        <v>147</v>
+        <v>3</v>
+      </c>
+      <c r="E103" t="s">
+        <v>84</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>22</v>
@@ -2645,56 +2665,76 @@
       <c r="K103" s="1"/>
     </row>
     <row r="104" spans="2:11">
-      <c r="F104" s="7"/>
-      <c r="G104" s="7"/>
-      <c r="H104" s="7"/>
-      <c r="I104" s="7"/>
-      <c r="J104" s="7"/>
-      <c r="K104" s="7"/>
+      <c r="D104">
+        <v>4</v>
+      </c>
+      <c r="E104" t="s">
+        <v>146</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
     </row>
     <row r="105" spans="2:11">
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
-      <c r="H105" s="7"/>
-      <c r="I105" s="7"/>
-      <c r="J105" s="7"/>
-      <c r="K105" s="7"/>
+      <c r="D105">
+        <v>5</v>
+      </c>
+      <c r="E105" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
     </row>
     <row r="106" spans="2:11">
-      <c r="C106" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D106" s="4"/>
-      <c r="E106" s="4" t="s">
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+    </row>
+    <row r="107" spans="2:11">
+      <c r="F107" s="7"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+    </row>
+    <row r="108" spans="2:11">
+      <c r="C108" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="2:11">
-      <c r="C107" s="4" t="s">
+    <row r="109" spans="2:11">
+      <c r="C109" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4" t="s">
+      <c r="D109" s="4"/>
+      <c r="E109" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="108" spans="2:11">
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
-      <c r="H108" s="7"/>
-      <c r="I108" s="7"/>
-    </row>
-    <row r="109" spans="2:11">
-      <c r="F109" s="7"/>
-      <c r="G109" s="7"/>
-      <c r="H109" s="7"/>
-      <c r="I109" s="7"/>
     </row>
     <row r="110" spans="2:11">
       <c r="F110" s="7"/>
-      <c r="G110" s="38"/>
-      <c r="H110" s="39"/>
-      <c r="I110" s="40"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
     </row>
     <row r="111" spans="2:11">
       <c r="F111" s="7"/>
@@ -2704,15 +2744,21 @@
     </row>
     <row r="112" spans="2:11">
       <c r="F112" s="7"/>
-      <c r="G112" s="7"/>
-      <c r="H112" s="7"/>
-      <c r="I112" s="7"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="39"/>
+      <c r="I112" s="40"/>
     </row>
     <row r="113" spans="6:9">
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
+    </row>
+    <row r="114" spans="6:9">
+      <c r="F114" s="7"/>
+      <c r="G114" s="7"/>
+      <c r="H114" s="7"/>
+      <c r="I114" s="7"/>
     </row>
     <row r="1048576" spans="6:6">
       <c r="F1048576" s="1"/>

</xml_diff>